<commit_message>
updates to sequential direction to better handle in-lake movement
</commit_message>
<xml_diff>
--- a/FDS_2025/output_tables/Slana_results_compiled.xlsx
+++ b/FDS_2025/output_tables/Slana_results_compiled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbtyers\Documents\Current Projects\Slana_whitefish_telemetry\FDS_2025\output_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605B2F5F-C439-4946-B439-9694B09B36B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977F0BCA-2975-4A7E-A96B-848C83EFFDC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-3780" windowWidth="38640" windowHeight="21120" xr2:uid="{E43D4DBE-05CA-4FA7-8C3B-7C2E9B1C5115}"/>
+    <workbookView xWindow="-38520" yWindow="-3780" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{E43D4DBE-05CA-4FA7-8C3B-7C2E9B1C5115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequential Distance" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5360" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5374" uniqueCount="137">
   <si>
     <t>0 to 1</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Survival state</t>
+  </si>
+  <si>
+    <t>in-lake</t>
   </si>
 </sst>
 </file>
@@ -931,14 +934,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
@@ -1318,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC5B40F8-2775-48E2-8541-92DC2FC8031F}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
   </sheetViews>
@@ -5560,7 +5560,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D8C4FF-3419-492E-98FD-BF9A984242DF}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -5792,19 +5794,19 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H6" t="s">
         <v>13</v>
@@ -5842,10 +5844,10 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G7" t="s">
         <v>13</v>
@@ -6018,16 +6020,16 @@
         <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I11" t="s">
         <v>13</v>
@@ -6232,13 +6234,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -6265,7 +6267,7 @@
         <v>15</v>
       </c>
       <c r="N16" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
@@ -6276,22 +6278,22 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G17" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I17" t="s">
         <v>13</v>
@@ -6329,7 +6331,7 @@
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G18" t="s">
         <v>13</v>
@@ -6373,7 +6375,7 @@
         <v>13</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G19" t="s">
         <v>13</v>
@@ -6452,13 +6454,13 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
@@ -6546,16 +6548,16 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G23" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I23" t="s">
         <v>13</v>
@@ -6570,10 +6572,10 @@
         <v>13</v>
       </c>
       <c r="M23" t="s">
-        <v>15</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="N23" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
@@ -6634,7 +6636,7 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
@@ -6687,7 +6689,7 @@
         <v>13</v>
       </c>
       <c r="H26" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I26" t="s">
         <v>14</v>
@@ -6722,7 +6724,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
@@ -6737,7 +6739,7 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K27" t="s">
         <v>13</v>
@@ -6757,7 +6759,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -6772,7 +6774,7 @@
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H28" t="s">
         <v>13</v>
@@ -6804,22 +6806,22 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G29" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I29" t="s">
         <v>13</v>
@@ -6834,10 +6836,10 @@
         <v>13</v>
       </c>
       <c r="M29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="N29" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
@@ -6854,22 +6856,22 @@
         <v>13</v>
       </c>
       <c r="E30" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G30" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I30" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="J30" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K30" t="s">
         <v>13</v>
@@ -6901,7 +6903,7 @@
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G31" t="s">
         <v>14</v>
@@ -6942,13 +6944,13 @@
         <v>13</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G32" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H32" t="s">
         <v>13</v>
@@ -7021,22 +7023,22 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H34" t="s">
         <v>13</v>
@@ -7124,7 +7126,7 @@
         <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H36" t="s">
         <v>13</v>
@@ -7159,16 +7161,16 @@
         <v>15</v>
       </c>
       <c r="D37" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="F37" t="s">
+        <v>136</v>
       </c>
       <c r="G37" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H37" t="s">
         <v>13</v>
@@ -7206,7 +7208,7 @@
         <v>13</v>
       </c>
       <c r="E38" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
@@ -7241,7 +7243,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
         <v>14</v>
@@ -7250,13 +7252,13 @@
         <v>15</v>
       </c>
       <c r="E39" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H39" t="s">
         <v>13</v>
@@ -7335,10 +7337,10 @@
         <v>15</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E41" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
@@ -7382,16 +7384,16 @@
         <v>13</v>
       </c>
       <c r="E42" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="F42" t="s">
+        <v>136</v>
       </c>
       <c r="G42" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I42" t="s">
         <v>13</v>
@@ -7417,7 +7419,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
         <v>13</v>
@@ -7470,13 +7472,13 @@
         <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F44" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H44" t="s">
         <v>13</v>
@@ -7599,16 +7601,16 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E47" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="F47" t="s">
+        <v>136</v>
       </c>
       <c r="G47" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H47" t="s">
         <v>13</v>
@@ -7617,7 +7619,7 @@
         <v>13</v>
       </c>
       <c r="J47" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K47" t="s">
         <v>13</v>
@@ -7637,7 +7639,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
         <v>13</v>
@@ -7646,7 +7648,7 @@
         <v>13</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
@@ -7725,25 +7727,25 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
+      <c r="D50" t="s">
+        <v>136</v>
+      </c>
+      <c r="E50" t="s">
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H50" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I50" t="s">
         <v>13</v>
@@ -7752,7 +7754,7 @@
         <v>13</v>
       </c>
       <c r="K50" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="L50" t="s">
         <v>13</v>
@@ -7781,16 +7783,16 @@
         <v>13</v>
       </c>
       <c r="F51" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H51" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I51" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="J51" t="s">
         <v>13</v>
@@ -7802,10 +7804,10 @@
         <v>13</v>
       </c>
       <c r="M51" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="N51" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35">
@@ -7822,22 +7824,22 @@
         <v>13</v>
       </c>
       <c r="E52" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F52" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H52" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I52" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J52" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K52" t="s">
         <v>13</v>
@@ -7915,8 +7917,8 @@
       <c r="F54" t="s">
         <v>13</v>
       </c>
-      <c r="G54">
-        <v>0</v>
+      <c r="G54" t="s">
+        <v>136</v>
       </c>
       <c r="H54" t="s">
         <v>13</v>
@@ -7947,17 +7949,17 @@
       <c r="B55" t="s">
         <v>15</v>
       </c>
-      <c r="C55">
-        <v>0</v>
+      <c r="C55" t="s">
+        <v>136</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E55" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F55" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G55" t="s">
         <v>13</v>
@@ -8007,13 +8009,13 @@
         <v>13</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I56" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J56" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="K56" t="s">
         <v>13</v>
@@ -8036,37 +8038,37 @@
         <v>15</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E57" t="s">
-        <v>14</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="F57" t="s">
+        <v>136</v>
       </c>
       <c r="G57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H57" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J57" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="L57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="M57" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="N57" t="s">
         <v>13</v>
@@ -8133,7 +8135,7 @@
         <v>15</v>
       </c>
       <c r="F59" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G59" t="s">
         <v>13</v>
@@ -8174,13 +8176,13 @@
         <v>13</v>
       </c>
       <c r="E60" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F60" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G60" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H60" t="s">
         <v>14</v>
@@ -8218,16 +8220,16 @@
         <v>13</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F61" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G61" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H61" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I61" t="s">
         <v>13</v>
@@ -8253,7 +8255,7 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
         <v>13</v>
@@ -8262,22 +8264,22 @@
         <v>13</v>
       </c>
       <c r="E62" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G62" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H62" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I62" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J62" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="K62" t="s">
         <v>13</v>
@@ -8438,19 +8440,19 @@
         <v>15</v>
       </c>
       <c r="E66" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F66" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G66" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H66" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I66" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J66" t="s">
         <v>13</v>
@@ -8520,16 +8522,16 @@
         <v>15</v>
       </c>
       <c r="C68" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E68" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F68" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G68" t="s">
         <v>14</v>
@@ -8613,14 +8615,14 @@
       <c r="D70" t="s">
         <v>13</v>
       </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
+      <c r="E70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
+        <v>136</v>
       </c>
       <c r="G70" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H70" t="s">
         <v>13</v>
@@ -8658,10 +8660,10 @@
         <v>13</v>
       </c>
       <c r="E71" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F71" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G71" t="s">
         <v>13</v>
@@ -8699,10 +8701,10 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E72" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
@@ -8743,13 +8745,13 @@
         <v>14</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E73" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F73" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G73" t="s">
         <v>13</v>
@@ -8790,16 +8792,16 @@
         <v>13</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F74" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G74" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="H74" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I74" t="s">
         <v>13</v>
@@ -8913,7 +8915,7 @@
         <v>79</v>
       </c>
       <c r="B77" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C77" t="s">
         <v>14</v>
@@ -8922,25 +8924,25 @@
         <v>15</v>
       </c>
       <c r="E77" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F77" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G77" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H77" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I77" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="J77" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="K77" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="L77" t="s">
         <v>13</v>
@@ -8960,13 +8962,13 @@
         <v>15</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="E78" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F78" t="s">
         <v>13</v>
@@ -9013,10 +9015,10 @@
         <v>13</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G79" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H79" t="s">
         <v>13</v>
@@ -9098,7 +9100,7 @@
         <v>15</v>
       </c>
       <c r="E81" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F81" t="s">
         <v>13</v>
@@ -9186,22 +9188,22 @@
         <v>15</v>
       </c>
       <c r="E83" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F83" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G83" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H83" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I83" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J83" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K83" t="s">
         <v>13</v>
@@ -9210,10 +9212,10 @@
         <v>13</v>
       </c>
       <c r="M83" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="N83" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.35">
@@ -9224,7 +9226,7 @@
         <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D84" t="s">
         <v>13</v>
@@ -9315,19 +9317,19 @@
         <v>14</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E86" t="s">
-        <v>15</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
+        <v>136</v>
+      </c>
+      <c r="F86" t="s">
+        <v>136</v>
       </c>
       <c r="G86" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H86" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I86" t="s">
         <v>13</v>
@@ -9361,8 +9363,8 @@
       <c r="D87" t="s">
         <v>15</v>
       </c>
-      <c r="E87">
-        <v>0</v>
+      <c r="E87" t="s">
+        <v>136</v>
       </c>
       <c r="F87" t="s">
         <v>13</v>
@@ -9371,13 +9373,13 @@
         <v>13</v>
       </c>
       <c r="H87" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I87" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="J87" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K87" t="s">
         <v>13</v>
@@ -9406,25 +9408,25 @@
         <v>15</v>
       </c>
       <c r="E88" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F88" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="G88" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H88" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I88" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="J88" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="K88" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="L88" t="s">
         <v>13</v>
@@ -9450,7 +9452,7 @@
         <v>15</v>
       </c>
       <c r="E89" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
@@ -9626,16 +9628,16 @@
         <v>15</v>
       </c>
       <c r="E93" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F93" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G93" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="H93" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="I93" t="s">
         <v>13</v>
@@ -9653,7 +9655,7 @@
         <v>13</v>
       </c>
       <c r="N93" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.35">
@@ -9670,7 +9672,7 @@
         <v>15</v>
       </c>
       <c r="E94" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="F94" t="s">
         <v>13</v>
@@ -9679,7 +9681,7 @@
         <v>13</v>
       </c>
       <c r="H94" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="I94" t="s">
         <v>13</v>
@@ -9707,17 +9709,17 @@
       <c r="B95" t="s">
         <v>15</v>
       </c>
-      <c r="C95">
-        <v>0</v>
+      <c r="C95" t="s">
+        <v>136</v>
       </c>
       <c r="D95" t="s">
-        <v>15</v>
+        <v>136</v>
       </c>
       <c r="E95" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="F95" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="G95" t="s">
         <v>14</v>
@@ -75624,290 +75626,278 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>45581</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="6">
+      <c r="E2" s="2">
         <v>0.99695301776791201</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="2">
         <v>9.1687458455723802E-3</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="2">
         <v>0.96800510995060196</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="2">
         <v>0.99999317289745204</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>45589</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6">
+      <c r="E3" s="2">
         <v>0.95431036979817596</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="2">
         <v>2.63667272845821E-2</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="2">
         <v>0.88626150897796596</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="2">
         <v>0.98733694659139704</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>45597</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6">
+      <c r="E4" s="2">
         <v>0.96161968746709503</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="2">
         <v>3.7058776921228997E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="2">
         <v>0.85708560238284204</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="2">
         <v>0.99641855587872796</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>45653</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6">
+      <c r="E5" s="2">
         <v>0.71583560178791505</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="2">
         <v>8.7271296091745804E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="2">
         <v>0.52525027047097705</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <v>0.86607771891878105</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>130</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>45733</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6">
+      <c r="E6" s="2">
         <v>0.64776102524963897</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <v>0.11252498180327</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="2">
         <v>0.413059769235533</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="2">
         <v>0.84111741346982805</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="1">
         <v>45796</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6">
+      <c r="E7" s="2">
         <v>0.85043773706222403</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="2">
         <v>8.9055497971779807E-2</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="2">
         <v>0.63179735270556503</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="2">
         <v>0.96914207408761899</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="1">
         <v>45819</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6">
+      <c r="E8" s="2">
         <v>0.70785921602109203</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="2">
         <v>0.11426544841339401</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="2">
         <v>0.45517375832309898</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="2">
         <v>0.89266942614023403</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="1">
         <v>45860</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6">
+      <c r="E9" s="2">
         <v>0.81018292207457199</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <v>0.111684426539229</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="2">
         <v>0.53534265940068904</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="2">
         <v>0.96129570033280398</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>129</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="1">
         <v>45908</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6">
+      <c r="E10" s="2">
         <v>0.73593898860743301</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>0.14104682813251601</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="2">
         <v>0.40731435549468997</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="2">
         <v>0.94131956516761395</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="1">
         <v>45924</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>0.70171938709634696</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="2">
         <v>0.15651621377144601</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="2">
         <v>0.34561788407342298</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="2">
         <v>0.93736020958613298</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>130</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="1">
         <v>45940</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
         <v>0.95879425000865903</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="2">
         <v>0.10329434717190999</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="2">
         <v>0.62954019179594201</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="2">
         <v>0.99990758338285202</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>130</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="1">
         <v>45952</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
         <v>0.95635364336780004</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>0.104473296541442</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="2">
         <v>0.62071528491987304</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="2">
         <v>0.99991289073227596</v>
       </c>
     </row>
@@ -75918,308 +75908,296 @@
       <c r="B14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>45959</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="8">
+      <c r="E14" s="5">
         <v>0.92987592480540604</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="5">
         <v>0.14828504690880201</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <v>0.46104272003445501</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="5">
         <v>0.99983773976650403</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>129</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>131</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="1">
         <v>45581</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6">
+      <c r="E15" s="2">
         <v>0.988947068630049</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="2">
         <v>3.1395468141543301E-2</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="2">
         <v>0.88678768756437198</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="2">
         <v>0.99997601734070096</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>131</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="1">
         <v>45589</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6">
+      <c r="E16" s="2">
         <v>0.99145307673934502</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="2">
         <v>2.58944600054626E-2</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="2">
         <v>0.90646607736519702</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="2">
         <v>0.99998212695133404</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
         <v>129</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>131</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="1">
         <v>45597</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6">
+      <c r="E17" s="2">
         <v>0.99111944288660903</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="2">
         <v>1.7975255218011001E-2</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="2">
         <v>0.93660149299727902</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="2">
         <v>0.99997746071449101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>129</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>131</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="1">
         <v>45653</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6">
+      <c r="E18" s="2">
         <v>0.96766541038155096</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="2">
         <v>2.5831520304154899E-2</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="2">
         <v>0.89840522353005303</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="2">
         <v>0.99616410983784098</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="A19" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>131</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="1">
         <v>45733</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6">
+      <c r="E19" s="2">
         <v>0.84290157659906995</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="2">
         <v>4.8251332858475098E-2</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="2">
         <v>0.73564761114847399</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="2">
         <v>0.92093574048608595</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>129</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>131</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="1">
         <v>45796</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="6">
+      <c r="E20" s="2">
         <v>0.94027624628287798</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="2">
         <v>3.8970630465610299E-2</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="2">
         <v>0.83862931992774403</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="2">
         <v>0.98830754674497101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="A21" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="1">
         <v>45819</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="6">
+      <c r="E21" s="2">
         <v>0.925868768855164</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="2">
         <v>5.8907257341636897E-2</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="2">
         <v>0.77065306733991101</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="2">
         <v>0.99203403030305404</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>129</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>131</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="1">
         <v>45860</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6">
+      <c r="E22" s="2">
         <v>0.67454678168299698</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="2">
         <v>8.7905288667515805E-2</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="2">
         <v>0.493449246162315</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="2">
         <v>0.83373428544164097</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>129</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>131</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="1">
         <v>45908</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6">
+      <c r="E23" s="2">
         <v>0.93303852916115204</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="2">
         <v>6.1063178712169403E-2</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="2">
         <v>0.76534807791402504</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="2">
         <v>0.99384766143655001</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" t="s">
         <v>129</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="1">
         <v>45924</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="6">
+      <c r="E24" s="2">
         <v>0.78573573106027905</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="2">
         <v>0.102382094899222</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="2">
         <v>0.55092346241897305</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="2">
         <v>0.93875928057899904</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>131</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="1">
         <v>45940</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6">
+      <c r="E25" s="2">
         <v>0.78508590113978305</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="2">
         <v>0.121370869303863</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="2">
         <v>0.497287071425908</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="2">
         <v>0.95507229222674295</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="1">
         <v>45952</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6">
+      <c r="E26" s="2">
         <v>0.97340428739596097</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="2">
         <v>7.4023456876271598E-2</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="2">
         <v>0.73559362385447002</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="2">
         <v>0.99995168238147303</v>
       </c>
     </row>
@@ -76230,44 +76208,43 @@
       <c r="B27" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>45959</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="8">
+      <c r="E27" s="5">
         <v>0.96785770092184198</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="5">
         <v>8.2542738493500606E-2</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="5">
         <v>0.69679150363304598</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="5">
         <v>0.99994286027553103</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" t="s">
         <v>132</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>130</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="s">
+      <c r="D28" t="s">
         <v>133</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="2">
         <v>0.89331166174637699</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="2">
         <v>1.9993737957600601E-2</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="2">
         <v>0.85010486040631195</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="2">
         <v>0.92764498534861095</v>
       </c>
     </row>
@@ -76282,40 +76259,39 @@
       <c r="D29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="5">
         <v>0.82568565257693005</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="5">
         <v>2.3976302633124599E-2</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="5">
         <v>0.77502843517424402</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="5">
         <v>0.86854455106020001</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="A30" t="s">
         <v>132</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>131</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="s">
+      <c r="D30" t="s">
         <v>133</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="2">
         <v>0.69146279031602698</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="2">
         <v>3.1038518937816E-2</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="2">
         <v>0.62939957294096105</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="2">
         <v>0.75011620847649296</v>
       </c>
     </row>
@@ -76330,16 +76306,16 @@
       <c r="D31" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E31" s="8">
+      <c r="E31" s="5">
         <v>0.83359828905578903</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="5">
         <v>2.0831781591897001E-2</v>
       </c>
-      <c r="G31" s="8">
+      <c r="G31" s="5">
         <v>0.789986313403786</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="5">
         <v>0.87242843429623596</v>
       </c>
     </row>

</xml_diff>